<commit_message>
Implemented load and get products
</commit_message>
<xml_diff>
--- a/UploadSheet.xlsx
+++ b/UploadSheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\50204512\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mazok\Documents\GitHub\TCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75419800-4503-4CA6-BBE5-486835E42433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -93,12 +94,30 @@
   </si>
   <si>
     <t>ServingSize</t>
+  </si>
+  <si>
+    <t>PELOTE</t>
+  </si>
+  <si>
+    <t>TBA</t>
+  </si>
+  <si>
+    <t>generic_thumb.jpg</t>
+  </si>
+  <si>
+    <t>generic_cover.jpg</t>
+  </si>
+  <si>
+    <t>0kcal</t>
+  </si>
+  <si>
+    <t>0g</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -136,9 +155,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,11 +438,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AA1"/>
+      <selection activeCell="I2" sqref="I2:W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,6 +522,77 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>